<commit_message>
Improve Cause & Effect matrix formatting
- Removed yellow P&ID cells from effect columns (row 4)
- Added label column (G) between CAUSE and EFFECT sections
- Separated effect headers into two rows:
  - Row 1: Service descriptions (e.g., "Fire Alarm Zone 1")
  - Row 2: Tag numbers (e.g., "B3:0/0")
- Column G now contains labels "EFFECT" and "Tag No"
- Improved readability with clearer structure
- Increased effect column width to 20 for better text display
</commit_message>
<xml_diff>
--- a/Cause_Effect_Output.xlsx
+++ b/Cause_Effect_Output.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +27,14 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="9"/>
     </font>
     <font>
       <sz val="9"/>
@@ -70,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -78,13 +86,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -473,20 +484,21 @@
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="18" customWidth="1" min="9" max="9"/>
-    <col width="18" customWidth="1" min="10" max="10"/>
-    <col width="18" customWidth="1" min="11" max="11"/>
-    <col width="18" customWidth="1" min="12" max="12"/>
-    <col width="18" customWidth="1" min="13" max="13"/>
-    <col width="18" customWidth="1" min="14" max="14"/>
-    <col width="18" customWidth="1" min="15" max="15"/>
-    <col width="18" customWidth="1" min="16" max="16"/>
-    <col width="18" customWidth="1" min="17" max="17"/>
-    <col width="18" customWidth="1" min="18" max="18"/>
-    <col width="18" customWidth="1" min="19" max="19"/>
-    <col width="18" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
+    <col width="20" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -501,20 +513,76 @@
           <t>EFFECT</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr"/>
-      <c r="I1" s="1" t="inlineStr"/>
-      <c r="J1" s="1" t="inlineStr"/>
-      <c r="K1" s="1" t="inlineStr"/>
-      <c r="L1" s="1" t="inlineStr"/>
-      <c r="M1" s="1" t="inlineStr"/>
-      <c r="N1" s="1" t="inlineStr"/>
-      <c r="O1" s="1" t="inlineStr"/>
-      <c r="P1" s="1" t="inlineStr"/>
-      <c r="Q1" s="1" t="inlineStr"/>
-      <c r="R1" s="1" t="inlineStr"/>
-      <c r="S1" s="1" t="inlineStr"/>
-      <c r="T1" s="1" t="inlineStr"/>
-      <c r="U1" t="inlineStr"/>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Fire Alarm Zone 1</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Fire Eye Failure Warning</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Strobe Light On</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Strobe Light On</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Fire Alarm Zone 2</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Strobe Light On</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>Plant ESD</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>Plant ESD</t>
+        </is>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>Plant ESD</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="inlineStr">
+        <is>
+          <t>Plant ESD</t>
+        </is>
+      </c>
+      <c r="R1" s="2" t="inlineStr">
+        <is>
+          <t>Plant ESD</t>
+        </is>
+      </c>
+      <c r="S1" s="2" t="inlineStr">
+        <is>
+          <t>Plant ESD</t>
+        </is>
+      </c>
+      <c r="T1" s="2" t="inlineStr">
+        <is>
+          <t>ESD Alarm to Office PLC</t>
+        </is>
+      </c>
+      <c r="U1" s="2" t="inlineStr">
+        <is>
+          <t>Deluge Valve Zone 2 Open</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" t="inlineStr"/>
@@ -523,120 +591,111 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>B3:0/0
-Fire Alarm Zone 1</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>B3:0/8
-Fire Eye Failure Warning</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>B3:0/9
-Strobe Light On</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>B3:0/10
-Strobe Light On</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>B3:0/11
-Fire Alarm Zone 2</t>
-        </is>
-      </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>B3:0/13
-Strobe Light On</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>B3:2/0
-Plant ESD</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>B3:2/4
-Plant ESD</t>
-        </is>
-      </c>
-      <c r="O2" s="2" t="inlineStr">
-        <is>
-          <t>B3:2/8
-Plant ESD</t>
-        </is>
-      </c>
-      <c r="P2" s="2" t="inlineStr">
-        <is>
-          <t>B3:2/9
-Plant ESD</t>
-        </is>
-      </c>
-      <c r="Q2" s="2" t="inlineStr">
-        <is>
-          <t>B3:2/10
-Plant ESD</t>
-        </is>
-      </c>
-      <c r="R2" s="2" t="inlineStr">
-        <is>
-          <t>B3:2/13
-Plant ESD</t>
-        </is>
-      </c>
-      <c r="S2" s="2" t="inlineStr">
-        <is>
-          <t>B3:10/0
-ESD Alarm to Office PLC</t>
-        </is>
-      </c>
-      <c r="T2" s="2" t="inlineStr">
-        <is>
-          <t>O:0/0
-Deluge Valve Zone 2 Open</t>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>Tag No</t>
+        </is>
+      </c>
+      <c r="H2" s="4" t="inlineStr">
+        <is>
+          <t>B3:0/0</t>
+        </is>
+      </c>
+      <c r="I2" s="4" t="inlineStr">
+        <is>
+          <t>B3:0/8</t>
+        </is>
+      </c>
+      <c r="J2" s="4" t="inlineStr">
+        <is>
+          <t>B3:0/9</t>
+        </is>
+      </c>
+      <c r="K2" s="4" t="inlineStr">
+        <is>
+          <t>B3:0/10</t>
+        </is>
+      </c>
+      <c r="L2" s="4" t="inlineStr">
+        <is>
+          <t>B3:0/11</t>
+        </is>
+      </c>
+      <c r="M2" s="4" t="inlineStr">
+        <is>
+          <t>B3:0/13</t>
+        </is>
+      </c>
+      <c r="N2" s="4" t="inlineStr">
+        <is>
+          <t>B3:2/0</t>
+        </is>
+      </c>
+      <c r="O2" s="4" t="inlineStr">
+        <is>
+          <t>B3:2/4</t>
+        </is>
+      </c>
+      <c r="P2" s="4" t="inlineStr">
+        <is>
+          <t>B3:2/8</t>
+        </is>
+      </c>
+      <c r="Q2" s="4" t="inlineStr">
+        <is>
+          <t>B3:2/9</t>
+        </is>
+      </c>
+      <c r="R2" s="4" t="inlineStr">
+        <is>
+          <t>B3:2/10</t>
+        </is>
+      </c>
+      <c r="S2" s="4" t="inlineStr">
+        <is>
+          <t>B3:2/13</t>
+        </is>
+      </c>
+      <c r="T2" s="4" t="inlineStr">
+        <is>
+          <t>B3:10/0</t>
+        </is>
+      </c>
+      <c r="U2" s="4" t="inlineStr">
+        <is>
+          <t>O:0/0</t>
         </is>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Interlock
 No</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>Tag No</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C3" s="5" t="inlineStr">
         <is>
           <t>Service Description</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D3" s="5" t="inlineStr">
         <is>
           <t>Range</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E3" s="5" t="inlineStr">
         <is>
           <t>Pre-Trip
 (H or L)</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="5" t="inlineStr">
         <is>
           <t>Trip
 (HH or LL)</t>
@@ -656,424 +715,370 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>CAUSE</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="I4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="J4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="K4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="L4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="M4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="N4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="O4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="P4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="Q4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="R4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="S4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
-      <c r="T4" s="5" t="inlineStr">
-        <is>
-          <t>P &amp; ID</t>
-        </is>
-      </c>
+      <c r="B4" s="7" t="inlineStr"/>
+      <c r="C4" s="7" t="inlineStr"/>
+      <c r="D4" s="7" t="inlineStr"/>
+      <c r="E4" s="7" t="inlineStr"/>
+      <c r="F4" s="7" t="inlineStr"/>
+      <c r="G4" s="7" t="inlineStr"/>
+      <c r="H4" s="7" t="inlineStr"/>
+      <c r="I4" s="7" t="inlineStr"/>
+      <c r="J4" s="7" t="inlineStr"/>
+      <c r="K4" s="7" t="inlineStr"/>
+      <c r="L4" s="7" t="inlineStr"/>
+      <c r="M4" s="7" t="inlineStr"/>
+      <c r="N4" s="7" t="inlineStr"/>
+      <c r="O4" s="7" t="inlineStr"/>
+      <c r="P4" s="7" t="inlineStr"/>
+      <c r="Q4" s="7" t="inlineStr"/>
+      <c r="R4" s="7" t="inlineStr"/>
+      <c r="S4" s="7" t="inlineStr"/>
+      <c r="T4" s="7" t="inlineStr"/>
+      <c r="U4" s="7" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>I-1</t>
         </is>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>B14:0/3</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" s="7" t="inlineStr">
         <is>
           <t>Plant ESD</t>
         </is>
       </c>
-      <c r="D5" s="6" t="inlineStr"/>
-      <c r="E5" s="6" t="inlineStr"/>
-      <c r="F5" s="6" t="inlineStr"/>
+      <c r="D5" s="7" t="inlineStr"/>
+      <c r="E5" s="7" t="inlineStr"/>
+      <c r="F5" s="7" t="inlineStr"/>
       <c r="G5" s="7" t="inlineStr"/>
-      <c r="H5" s="7" t="inlineStr"/>
-      <c r="I5" s="7" t="inlineStr"/>
-      <c r="J5" s="7" t="inlineStr"/>
-      <c r="K5" s="7" t="inlineStr"/>
-      <c r="L5" s="7" t="inlineStr"/>
-      <c r="M5" s="7" t="inlineStr"/>
-      <c r="N5" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="O5" s="7" t="inlineStr"/>
-      <c r="P5" s="7" t="inlineStr"/>
-      <c r="Q5" s="7" t="inlineStr"/>
-      <c r="R5" s="7" t="inlineStr"/>
-      <c r="S5" s="7" t="inlineStr"/>
-      <c r="T5" s="7" t="inlineStr"/>
-      <c r="U5" s="7" t="n"/>
+      <c r="H5" s="8" t="inlineStr"/>
+      <c r="I5" s="8" t="inlineStr"/>
+      <c r="J5" s="8" t="inlineStr"/>
+      <c r="K5" s="8" t="inlineStr"/>
+      <c r="L5" s="8" t="inlineStr"/>
+      <c r="M5" s="8" t="inlineStr"/>
+      <c r="N5" s="8" t="inlineStr"/>
+      <c r="O5" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P5" s="8" t="inlineStr"/>
+      <c r="Q5" s="8" t="inlineStr"/>
+      <c r="R5" s="8" t="inlineStr"/>
+      <c r="S5" s="8" t="inlineStr"/>
+      <c r="T5" s="8" t="inlineStr"/>
+      <c r="U5" s="8" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>I-2</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" s="7" t="inlineStr">
         <is>
           <t>I:0/1</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
+      <c r="C6" s="7" t="inlineStr">
         <is>
           <t>Pull Station 2 Zone 1</t>
         </is>
       </c>
-      <c r="D6" s="6" t="inlineStr"/>
-      <c r="E6" s="6" t="inlineStr"/>
-      <c r="F6" s="6" t="inlineStr"/>
-      <c r="G6" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H6" s="7" t="inlineStr"/>
-      <c r="I6" s="7" t="inlineStr"/>
-      <c r="J6" s="7" t="inlineStr"/>
-      <c r="K6" s="7" t="inlineStr"/>
-      <c r="L6" s="7" t="inlineStr"/>
-      <c r="M6" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N6" s="7" t="inlineStr"/>
-      <c r="O6" s="7" t="inlineStr"/>
-      <c r="P6" s="7" t="inlineStr"/>
-      <c r="Q6" s="7" t="inlineStr"/>
-      <c r="R6" s="7" t="inlineStr"/>
-      <c r="S6" s="7" t="inlineStr"/>
-      <c r="T6" s="7" t="inlineStr"/>
-      <c r="U6" s="7" t="n"/>
+      <c r="D6" s="7" t="inlineStr"/>
+      <c r="E6" s="7" t="inlineStr"/>
+      <c r="F6" s="7" t="inlineStr"/>
+      <c r="G6" s="7" t="inlineStr"/>
+      <c r="H6" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I6" s="8" t="inlineStr"/>
+      <c r="J6" s="8" t="inlineStr"/>
+      <c r="K6" s="8" t="inlineStr"/>
+      <c r="L6" s="8" t="inlineStr"/>
+      <c r="M6" s="8" t="inlineStr"/>
+      <c r="N6" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O6" s="8" t="inlineStr"/>
+      <c r="P6" s="8" t="inlineStr"/>
+      <c r="Q6" s="8" t="inlineStr"/>
+      <c r="R6" s="8" t="inlineStr"/>
+      <c r="S6" s="8" t="inlineStr"/>
+      <c r="T6" s="8" t="inlineStr"/>
+      <c r="U6" s="8" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>I-3</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" s="7" t="inlineStr">
         <is>
           <t>I:0/0</t>
         </is>
       </c>
-      <c r="C7" s="6" t="inlineStr">
+      <c r="C7" s="7" t="inlineStr">
         <is>
           <t>Pull Station 1 Zone 2</t>
         </is>
       </c>
-      <c r="D7" s="6" t="inlineStr"/>
-      <c r="E7" s="6" t="inlineStr"/>
-      <c r="F7" s="6" t="inlineStr"/>
+      <c r="D7" s="7" t="inlineStr"/>
+      <c r="E7" s="7" t="inlineStr"/>
+      <c r="F7" s="7" t="inlineStr"/>
       <c r="G7" s="7" t="inlineStr"/>
-      <c r="H7" s="7" t="inlineStr"/>
-      <c r="I7" s="7" t="inlineStr"/>
-      <c r="J7" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K7" s="7" t="inlineStr"/>
-      <c r="L7" s="7" t="inlineStr"/>
-      <c r="M7" s="7" t="inlineStr"/>
-      <c r="N7" s="7" t="inlineStr"/>
-      <c r="O7" s="7" t="inlineStr"/>
-      <c r="P7" s="7" t="inlineStr"/>
-      <c r="Q7" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="R7" s="7" t="inlineStr"/>
-      <c r="S7" s="7" t="inlineStr"/>
-      <c r="T7" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="U7" s="7" t="n"/>
+      <c r="H7" s="8" t="inlineStr"/>
+      <c r="I7" s="8" t="inlineStr"/>
+      <c r="J7" s="8" t="inlineStr"/>
+      <c r="K7" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L7" s="8" t="inlineStr"/>
+      <c r="M7" s="8" t="inlineStr"/>
+      <c r="N7" s="8" t="inlineStr"/>
+      <c r="O7" s="8" t="inlineStr"/>
+      <c r="P7" s="8" t="inlineStr"/>
+      <c r="Q7" s="8" t="inlineStr"/>
+      <c r="R7" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S7" s="8" t="inlineStr"/>
+      <c r="T7" s="8" t="inlineStr"/>
+      <c r="U7" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>I-4</t>
         </is>
       </c>
-      <c r="B8" s="6" t="inlineStr">
+      <c r="B8" s="7" t="inlineStr">
         <is>
           <t>B11:0/1</t>
         </is>
       </c>
-      <c r="C8" s="6" t="inlineStr">
+      <c r="C8" s="7" t="inlineStr">
         <is>
           <t>Pull Station 8 Zone 1</t>
         </is>
       </c>
-      <c r="D8" s="6" t="inlineStr"/>
-      <c r="E8" s="6" t="inlineStr"/>
-      <c r="F8" s="6" t="inlineStr"/>
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
-      <c r="J8" s="7" t="inlineStr"/>
-      <c r="K8" s="7" t="inlineStr"/>
-      <c r="L8" s="7" t="inlineStr"/>
-      <c r="M8" s="7" t="inlineStr"/>
-      <c r="N8" s="7" t="inlineStr"/>
-      <c r="O8" s="7" t="inlineStr"/>
-      <c r="P8" s="7" t="inlineStr"/>
-      <c r="Q8" s="7" t="inlineStr"/>
-      <c r="R8" s="7" t="inlineStr"/>
-      <c r="S8" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="T8" s="7" t="inlineStr"/>
-      <c r="U8" s="7" t="n"/>
+      <c r="H8" s="8" t="inlineStr"/>
+      <c r="I8" s="8" t="inlineStr"/>
+      <c r="J8" s="8" t="inlineStr"/>
+      <c r="K8" s="8" t="inlineStr"/>
+      <c r="L8" s="8" t="inlineStr"/>
+      <c r="M8" s="8" t="inlineStr"/>
+      <c r="N8" s="8" t="inlineStr"/>
+      <c r="O8" s="8" t="inlineStr"/>
+      <c r="P8" s="8" t="inlineStr"/>
+      <c r="Q8" s="8" t="inlineStr"/>
+      <c r="R8" s="8" t="inlineStr"/>
+      <c r="S8" s="8" t="inlineStr"/>
+      <c r="T8" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="U8" s="8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>I-5</t>
         </is>
       </c>
-      <c r="B9" s="6" t="inlineStr">
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>B14:0/2</t>
         </is>
       </c>
-      <c r="C9" s="6" t="inlineStr">
+      <c r="C9" s="7" t="inlineStr">
         <is>
           <t>Fire Alarm Zone 2</t>
         </is>
       </c>
-      <c r="D9" s="6" t="inlineStr"/>
-      <c r="E9" s="6" t="inlineStr"/>
-      <c r="F9" s="6" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="7" t="inlineStr"/>
-      <c r="J9" s="7" t="inlineStr"/>
-      <c r="K9" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L9" s="7" t="inlineStr"/>
-      <c r="M9" s="7" t="inlineStr"/>
-      <c r="N9" s="7" t="inlineStr"/>
-      <c r="O9" s="7" t="inlineStr"/>
-      <c r="P9" s="7" t="inlineStr"/>
-      <c r="Q9" s="7" t="inlineStr"/>
-      <c r="R9" s="7" t="inlineStr"/>
-      <c r="S9" s="7" t="inlineStr"/>
-      <c r="T9" s="7" t="inlineStr"/>
-      <c r="U9" s="7" t="n"/>
+      <c r="H9" s="8" t="inlineStr"/>
+      <c r="I9" s="8" t="inlineStr"/>
+      <c r="J9" s="8" t="inlineStr"/>
+      <c r="K9" s="8" t="inlineStr"/>
+      <c r="L9" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M9" s="8" t="inlineStr"/>
+      <c r="N9" s="8" t="inlineStr"/>
+      <c r="O9" s="8" t="inlineStr"/>
+      <c r="P9" s="8" t="inlineStr"/>
+      <c r="Q9" s="8" t="inlineStr"/>
+      <c r="R9" s="8" t="inlineStr"/>
+      <c r="S9" s="8" t="inlineStr"/>
+      <c r="T9" s="8" t="inlineStr"/>
+      <c r="U9" s="8" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="inlineStr">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>I-6</t>
         </is>
       </c>
-      <c r="B10" s="6" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>I:1/12</t>
         </is>
       </c>
-      <c r="C10" s="6" t="inlineStr">
+      <c r="C10" s="7" t="inlineStr">
         <is>
           <t>Fire Eye Failure Warning</t>
         </is>
       </c>
-      <c r="D10" s="6" t="inlineStr"/>
-      <c r="E10" s="6" t="inlineStr"/>
-      <c r="F10" s="6" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
-      <c r="J10" s="7" t="inlineStr"/>
-      <c r="K10" s="7" t="inlineStr"/>
-      <c r="L10" s="7" t="inlineStr"/>
-      <c r="M10" s="7" t="inlineStr"/>
-      <c r="N10" s="7" t="inlineStr"/>
-      <c r="O10" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P10" s="7" t="inlineStr"/>
-      <c r="Q10" s="7" t="inlineStr"/>
-      <c r="R10" s="7" t="inlineStr"/>
-      <c r="S10" s="7" t="inlineStr"/>
-      <c r="T10" s="7" t="inlineStr"/>
-      <c r="U10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr"/>
+      <c r="I10" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="J10" s="8" t="inlineStr"/>
+      <c r="K10" s="8" t="inlineStr"/>
+      <c r="L10" s="8" t="inlineStr"/>
+      <c r="M10" s="8" t="inlineStr"/>
+      <c r="N10" s="8" t="inlineStr"/>
+      <c r="O10" s="8" t="inlineStr"/>
+      <c r="P10" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q10" s="8" t="inlineStr"/>
+      <c r="R10" s="8" t="inlineStr"/>
+      <c r="S10" s="8" t="inlineStr"/>
+      <c r="T10" s="8" t="inlineStr"/>
+      <c r="U10" s="8" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="inlineStr">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>I-7</t>
         </is>
       </c>
-      <c r="B11" s="6" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>I:1/13</t>
         </is>
       </c>
-      <c r="C11" s="6" t="inlineStr">
+      <c r="C11" s="7" t="inlineStr">
         <is>
           <t>Strobe Light Trigger</t>
         </is>
       </c>
-      <c r="D11" s="6" t="inlineStr"/>
-      <c r="E11" s="6" t="inlineStr"/>
-      <c r="F11" s="6" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="7" t="inlineStr"/>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr"/>
-      <c r="K11" s="7" t="inlineStr"/>
-      <c r="L11" s="7" t="inlineStr"/>
-      <c r="M11" s="7" t="inlineStr"/>
-      <c r="N11" s="7" t="inlineStr"/>
-      <c r="O11" s="7" t="inlineStr"/>
-      <c r="P11" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="Q11" s="7" t="inlineStr"/>
-      <c r="R11" s="7" t="inlineStr"/>
-      <c r="S11" s="7" t="inlineStr"/>
-      <c r="T11" s="7" t="inlineStr"/>
-      <c r="U11" s="7" t="n"/>
+      <c r="H11" s="8" t="inlineStr"/>
+      <c r="I11" s="8" t="inlineStr"/>
+      <c r="J11" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K11" s="8" t="inlineStr"/>
+      <c r="L11" s="8" t="inlineStr"/>
+      <c r="M11" s="8" t="inlineStr"/>
+      <c r="N11" s="8" t="inlineStr"/>
+      <c r="O11" s="8" t="inlineStr"/>
+      <c r="P11" s="8" t="inlineStr"/>
+      <c r="Q11" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R11" s="8" t="inlineStr"/>
+      <c r="S11" s="8" t="inlineStr"/>
+      <c r="T11" s="8" t="inlineStr"/>
+      <c r="U11" s="8" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="inlineStr">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>I-8</t>
         </is>
       </c>
-      <c r="B12" s="6" t="inlineStr">
+      <c r="B12" s="7" t="inlineStr">
         <is>
           <t>I:1/15</t>
         </is>
       </c>
-      <c r="C12" s="6" t="inlineStr">
+      <c r="C12" s="7" t="inlineStr">
         <is>
           <t>Strobe Light Trigger</t>
         </is>
       </c>
-      <c r="D12" s="6" t="inlineStr"/>
-      <c r="E12" s="6" t="inlineStr"/>
-      <c r="F12" s="6" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
       <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="7" t="inlineStr"/>
-      <c r="I12" s="7" t="inlineStr"/>
-      <c r="J12" s="7" t="inlineStr"/>
-      <c r="K12" s="7" t="inlineStr"/>
-      <c r="L12" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M12" s="7" t="inlineStr"/>
-      <c r="N12" s="7" t="inlineStr"/>
-      <c r="O12" s="7" t="inlineStr"/>
-      <c r="P12" s="7" t="inlineStr"/>
-      <c r="Q12" s="7" t="inlineStr"/>
-      <c r="R12" s="8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="S12" s="7" t="inlineStr"/>
-      <c r="T12" s="7" t="inlineStr"/>
-      <c r="U12" s="7" t="n"/>
+      <c r="H12" s="8" t="inlineStr"/>
+      <c r="I12" s="8" t="inlineStr"/>
+      <c r="J12" s="8" t="inlineStr"/>
+      <c r="K12" s="8" t="inlineStr"/>
+      <c r="L12" s="8" t="inlineStr"/>
+      <c r="M12" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="N12" s="8" t="inlineStr"/>
+      <c r="O12" s="8" t="inlineStr"/>
+      <c r="P12" s="8" t="inlineStr"/>
+      <c r="Q12" s="8" t="inlineStr"/>
+      <c r="R12" s="8" t="inlineStr"/>
+      <c r="S12" s="9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="T12" s="8" t="inlineStr"/>
+      <c r="U12" s="8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>